<commit_message>
added comments and error page
</commit_message>
<xml_diff>
--- a/web/files/addresses.xlsx
+++ b/web/files/addresses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chubi/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CC2CE5C-CBA4-3748-9C87-4BE5775C39E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC618B61-37FE-C34A-878C-3F956EF2CF2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{5FA8674E-8526-F643-870D-213F9A27E6F4}"/>
   </bookViews>
@@ -34,15 +34,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
-    <t>street number</t>
-  </si>
-  <si>
-    <t>street name</t>
-  </si>
-  <si>
-    <t>apt number</t>
-  </si>
-  <si>
     <t>city</t>
   </si>
   <si>
@@ -68,6 +59,15 @@
   </si>
   <si>
     <t>St Petersburg</t>
+  </si>
+  <si>
+    <t>street_number</t>
+  </si>
+  <si>
+    <t>street_name</t>
+  </si>
+  <si>
+    <t>apt_number</t>
   </si>
 </sst>
 </file>
@@ -104,10 +104,9 @@
     </font>
     <font>
       <b/>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -118,12 +117,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -134,10 +148,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -455,7 +471,7 @@
   <dimension ref="A1:AH8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -467,30 +483,30 @@
     <col min="7" max="11" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="E1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="F1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
@@ -516,103 +532,103 @@
       <c r="AH1" s="2"/>
     </row>
     <row r="2" spans="1:34" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="5">
+      <c r="A2" s="4">
         <v>11829</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="6">
+      <c r="B2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="5">
         <v>33625</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
     </row>
     <row r="3" spans="1:34" ht="18" x14ac:dyDescent="0.2">
-      <c r="A3" s="5">
+      <c r="A3" s="4">
         <v>500</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="6">
+      <c r="B3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="5">
         <v>1204</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="6">
+      <c r="E3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="5">
         <v>33716</v>
       </c>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
     </row>
     <row r="4" spans="1:34" ht="18" x14ac:dyDescent="0.2">
-      <c r="A4" s="5">
+      <c r="A4" s="4">
         <v>10420</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="6">
-        <v>1210</v>
-      </c>
-      <c r="D4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="6">
+      <c r="C4" s="5">
+        <v>1201</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="5">
         <v>33612</v>
       </c>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
     </row>
     <row r="5" spans="1:34" ht="18" x14ac:dyDescent="0.2">
-      <c r="A5" s="5"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
     </row>
     <row r="6" spans="1:34" ht="18" x14ac:dyDescent="0.2">
-      <c r="A6" s="5"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
+      <c r="A6" s="4"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.2">
       <c r="B8" s="2"/>

</xml_diff>